<commit_message>
[DONE] Taula A4 actualitzada i corregit un bug.
</commit_message>
<xml_diff>
--- a/public/20220421_SUGGEREIX_Taula_A4.xlsx
+++ b/public/20220421_SUGGEREIX_Taula_A4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ficra.sharepoint.com/sites/SADSUGGEREIX/Materiales de clase/Doc_SAD_actualitzada/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="109" documentId="11_013BE0263988F37BD8F142E6F7ED0C930FC3E02C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E813CE32-6234-40EF-8B89-ADCDB3D7A7D9}"/>
+  <xr:revisionPtr revIDLastSave="137" documentId="11_013BE0263988F37BD8F142E6F7ED0C930FC3E02C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="48" xr10:uidLastSave="{6542F1C4-5895-4698-8DFF-033E1144DEC7}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="200">
   <si>
     <t>Taula A4. Mètodes de monitoratge</t>
   </si>
@@ -209,37 +209,6 @@
     <t>EN 1484; ISO 8245</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>NH</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>4</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>+</t>
-    </r>
-  </si>
-  <si>
     <t>I6</t>
   </si>
   <si>
@@ -259,37 +228,6 @@
   </si>
   <si>
     <t>ISO 6778</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>NO</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>3</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>-</t>
-    </r>
   </si>
   <si>
     <t>I7</t>
@@ -500,6 +438,18 @@
   </si>
   <si>
     <t>Munch 1995</t>
+  </si>
+  <si>
+    <t>Clorat</t>
+  </si>
+  <si>
+    <t>Djoukeng i Jensen 2016</t>
+  </si>
+  <si>
+    <t>Clorit</t>
+  </si>
+  <si>
+    <t>Bromat</t>
   </si>
   <si>
     <t>Clor lliure residual</t>
@@ -844,16 +794,91 @@
     <t>Electron capture detector</t>
   </si>
   <si>
-    <t>Clorat</t>
-  </si>
-  <si>
-    <t>Clorit</t>
-  </si>
-  <si>
-    <t>Bromat</t>
-  </si>
-  <si>
-    <t>Djoukeng i Jensen 2016</t>
+    <r>
+      <t>Amoni (NH</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Nitrat (NO</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>Zinc (Zn)</t>
+  </si>
+  <si>
+    <t>Níquel (Ni)</t>
+  </si>
+  <si>
+    <t>OT2</t>
+  </si>
+  <si>
+    <t>OT1</t>
+  </si>
+  <si>
+    <t>OT3</t>
+  </si>
+  <si>
+    <t>OT4</t>
+  </si>
+  <si>
+    <t>OT5</t>
   </si>
 </sst>
 </file>
@@ -1476,8 +1501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMJ77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1640,13 +1665,13 @@
     </row>
     <row r="10" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="C10" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>28</v>
@@ -1655,18 +1680,18 @@
         <v>11</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>37</v>
-      </c>
       <c r="C11" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>34</v>
@@ -1675,18 +1700,18 @@
         <v>11</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>37</v>
-      </c>
       <c r="C12" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>10</v>
@@ -1695,18 +1720,18 @@
         <v>11</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>44</v>
+        <v>192</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>28</v>
@@ -1715,18 +1740,18 @@
         <v>11</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>44</v>
+        <v>192</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>34</v>
@@ -1735,18 +1760,18 @@
         <v>11</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>44</v>
+        <v>192</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>10</v>
@@ -1755,38 +1780,38 @@
         <v>11</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>44</v>
+        <v>192</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>28</v>
@@ -1795,18 +1820,18 @@
         <v>11</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>52</v>
+        <v>193</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>28</v>
@@ -1815,18 +1840,18 @@
         <v>11</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>52</v>
+        <v>193</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>28</v>
@@ -1835,18 +1860,18 @@
         <v>11</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>60</v>
+        <v>194</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>28</v>
@@ -1855,18 +1880,18 @@
         <v>11</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>60</v>
+        <v>194</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>28</v>
@@ -1875,18 +1900,18 @@
         <v>11</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>60</v>
+        <v>194</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>28</v>
@@ -1895,198 +1920,198 @@
         <v>11</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>64</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>28</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>28</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>28</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>28</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>75</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>28</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>28</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>28</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>28</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>28</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>90</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>28</v>
@@ -2095,18 +2120,18 @@
         <v>11</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>94</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>28</v>
@@ -2115,38 +2140,38 @@
         <v>11</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>28</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>100</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>28</v>
@@ -2155,38 +2180,38 @@
         <v>11</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>28</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>103</v>
+        <v>100</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>195</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>28</v>
@@ -2195,18 +2220,18 @@
         <v>11</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="C38" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>107</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>28</v>
@@ -2217,33 +2242,33 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="B39" s="7" t="s">
-        <v>106</v>
+        <v>103</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>196</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>28</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="B40" s="7" t="s">
-        <v>8</v>
+        <v>107</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>197</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>28</v>
@@ -2252,18 +2277,18 @@
         <v>11</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>192</v>
+        <v>108</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="B41" s="7" t="s">
-        <v>8</v>
+        <v>109</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>198</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>28</v>
@@ -2272,18 +2297,18 @@
         <v>11</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>192</v>
+        <v>108</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="B42" s="7" t="s">
-        <v>8</v>
+        <v>110</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>199</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>28</v>
@@ -2292,18 +2317,18 @@
         <v>11</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>192</v>
+        <v>108</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>34</v>
@@ -2312,38 +2337,38 @@
         <v>11</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>34</v>
@@ -2352,59 +2377,59 @@
         <v>11</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="G47" s="7"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>28</v>
@@ -2413,18 +2438,18 @@
         <v>11</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>34</v>
@@ -2433,18 +2458,18 @@
         <v>11</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>34</v>
@@ -2453,58 +2478,58 @@
         <v>11</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>28</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="8" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>10</v>
@@ -2513,18 +2538,18 @@
         <v>11</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>10</v>
@@ -2533,18 +2558,18 @@
         <v>11</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>10</v>
@@ -2553,227 +2578,227 @@
         <v>11</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="8" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="8" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="8" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="8" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="8" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="8" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="8" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="8" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="8" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="8" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -2833,54 +2858,54 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>153</v>
-      </c>
       <c r="J3" s="2" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C4" s="23">
         <f>600/1000*14/18</f>
         <v>0.46666666666666667</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="F4" s="20">
         <f>C4*0.3</f>
@@ -2888,26 +2913,26 @@
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="1" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="I4" s="2"/>
     </row>
     <row r="5" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C5" s="23">
         <f>25000/1000*1/62*14</f>
         <v>5.6451612903225801</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>161</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>159</v>
       </c>
       <c r="F5" s="20">
         <f>C5*0.3</f>
@@ -2915,85 +2940,85 @@
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="1" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="I5" s="2"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C6" s="1">
         <v>30</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="F6" s="21">
         <f t="shared" ref="F6:F18" si="0">0.3*C6</f>
         <v>9</v>
       </c>
       <c r="G6" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>162</v>
-      </c>
       <c r="I6" s="1" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C7" s="1">
         <v>4</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="F7" s="21">
         <f t="shared" si="0"/>
         <v>1.2</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C8" s="1">
         <v>0.05</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="F8" s="4">
         <f t="shared" si="0"/>
@@ -3003,30 +3028,30 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C9" s="1">
         <v>0.1</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="F9" s="4">
         <f t="shared" si="0"/>
@@ -3036,30 +3061,30 @@
         <v>1.7100000000000001E-2</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C10" s="1">
         <v>88</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="F10" s="21">
         <f t="shared" si="0"/>
@@ -3069,27 +3094,27 @@
         <v>1E-3</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C11" s="1">
         <v>0.14000000000000001</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="F11" s="22">
         <f t="shared" si="0"/>
@@ -3099,57 +3124,57 @@
         <v>2.2800000000000001E-2</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C12" s="7">
         <v>29000</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="F12" s="4">
         <f t="shared" si="0"/>
         <v>8700</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C13" s="1">
         <v>3.7999999999999999E-2</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="F13" s="22">
         <f t="shared" si="0"/>
@@ -3159,27 +3184,27 @@
         <v>2.0999999999999999E-3</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C14" s="4">
         <v>87</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="F14" s="21">
         <f t="shared" si="0"/>
@@ -3189,27 +3214,27 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C15" s="1">
         <v>6.4999999999999997E-4</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="F15" s="10">
         <f t="shared" si="0"/>
@@ -3219,27 +3244,27 @@
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C16" s="1">
         <v>1.3</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="F16" s="20">
         <f t="shared" si="0"/>
@@ -3249,27 +3274,27 @@
         <v>0.13</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C17" s="18">
         <v>0.1</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="E17" s="19" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="F17" s="4">
         <f t="shared" si="0"/>
@@ -3280,27 +3305,27 @@
         <v>1E-3</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="I17" s="19" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C18" s="18">
         <v>2.5</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="E18" s="19" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="F18" s="4">
         <f t="shared" si="0"/>
@@ -3310,10 +3335,10 @@
         <v>1</v>
       </c>
       <c r="H18" s="19" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="I18" s="19" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -3435,71 +3460,71 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="15" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>
@@ -3508,21 +3533,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010042169B78D842A848BE799D251A5B2C6A" ma:contentTypeVersion="7" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="625099e38fc716cc4bb30b36cfa7c837">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="758674b2-73ae-44f0-9f19-d4ad379aa2ea" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c97fa59194b5c482d1d5e2dd6e3e6b4b" ns2:_="">
     <xsd:import namespace="758674b2-73ae-44f0-9f19-d4ad379aa2ea"/>
@@ -3686,31 +3696,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10B0E896-02C8-4516-A9C3-929A1F756C25}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="758674b2-73ae-44f0-9f19-d4ad379aa2ea"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A79B44E-F529-45E6-81AB-F32F26836690}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7F36E16F-DF1A-473A-AFD5-6F4950C7FD58}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3726,4 +3727,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10B0E896-02C8-4516-A9C3-929A1F756C25}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="758674b2-73ae-44f0-9f19-d4ad379aa2ea"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A79B44E-F529-45E6-81AB-F32F26836690}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>